<commit_message>
Enhance main.py with graceful shutdown handling and daemon thread management; add photo URL extraction in nodes.py. Update dependencies in pyproject.toml and uv.lock to include tabulate. Improve logging for thread management and processing interruptions.
</commit_message>
<xml_diff>
--- a/output/errors_extracted_profiles.xlsx
+++ b/output/errors_extracted_profiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>error_details</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>thread_id</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -463,7 +468,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/services/grant-and-project-development/our-people/tenley-burke', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 68, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/services/grant-and-project-development/our-people/tenley-burke\n'}</t>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/services/grant-and-project-development/our-people/tenley-burke', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/services/grant-and-project-development/our-people/tenley-burke\n'}</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
         </is>
       </c>
     </row>

</xml_diff>